<commit_message>
Added some stats to branch prediction results
</commit_message>
<xml_diff>
--- a/results/branchpredict.xlsx
+++ b/results/branchpredict.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="16">
   <si>
     <t>Indirect Branches</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Table Only</t>
+  </si>
+  <si>
+    <t>predict</t>
+  </si>
+  <si>
+    <t>mispred</t>
   </si>
 </sst>
 </file>
@@ -244,17 +250,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T62"/>
+  <dimension ref="A1:T75"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="17.3775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8214285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.515306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.0051020408163"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.9234693877551"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
   </cols>
@@ -597,7 +603,10 @@
         <f aca="false">D13/C13</f>
         <v>0.289279910003415</v>
       </c>
-      <c r="F13" s="4"/>
+      <c r="F13" s="4" t="n">
+        <f aca="false">AVERAGE(E10:E16)</f>
+        <v>0.184147805702677</v>
+      </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -846,7 +855,10 @@
         <f aca="false">D22/C22</f>
         <v>0.665562560261382</v>
       </c>
-      <c r="F22" s="4"/>
+      <c r="F22" s="4" t="n">
+        <f aca="false">AVERAGE(E18:E24)</f>
+        <v>0.499810007272695</v>
+      </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -974,7 +986,10 @@
         <f aca="false">D27/C27</f>
         <v>0.345010636012975</v>
       </c>
-      <c r="F27" s="4"/>
+      <c r="F27" s="4" t="n">
+        <f aca="false">AVERAGE(E26:E32)</f>
+        <v>0.185814541753639</v>
+      </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -1431,6 +1446,12 @@
       <c r="F47" s="6"/>
       <c r="N47" s="6"/>
       <c r="O47" s="6"/>
+      <c r="Q47" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="R47" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1"/>
@@ -1450,7 +1471,9 @@
         <v>0.289279910003415</v>
       </c>
       <c r="F48" s="6"/>
-      <c r="N48" s="6"/>
+      <c r="N48" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="O48" s="6"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1472,7 +1495,22 @@
       </c>
       <c r="F49" s="6"/>
       <c r="N49" s="6"/>
-      <c r="O49" s="6"/>
+      <c r="O49" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P49" s="0" t="n">
+        <v>31492889979</v>
+      </c>
+      <c r="Q49" s="0" t="n">
+        <f aca="false">P49-R49</f>
+        <v>28629447240</v>
+      </c>
+      <c r="R49" s="0" t="n">
+        <v>2863442739</v>
+      </c>
+      <c r="S49" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1"/>
@@ -1493,7 +1531,22 @@
       </c>
       <c r="F50" s="6"/>
       <c r="N50" s="6"/>
-      <c r="O50" s="6"/>
+      <c r="O50" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="P50" s="0" t="n">
+        <v>31492889979</v>
+      </c>
+      <c r="Q50" s="0" t="n">
+        <f aca="false">P50-R50</f>
+        <v>14314985800</v>
+      </c>
+      <c r="R50" s="0" t="n">
+        <v>17177904179</v>
+      </c>
+      <c r="S50" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
@@ -1516,7 +1569,22 @@
       </c>
       <c r="F51" s="6"/>
       <c r="N51" s="6"/>
-      <c r="O51" s="6"/>
+      <c r="O51" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P51" s="0" t="n">
+        <v>31492889979</v>
+      </c>
+      <c r="Q51" s="0" t="n">
+        <f aca="false">P51-R51</f>
+        <v>28629447240</v>
+      </c>
+      <c r="R51" s="0" t="n">
+        <v>2863442739</v>
+      </c>
+      <c r="S51" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1"/>
@@ -1536,7 +1604,9 @@
         <v>0.227268270845914</v>
       </c>
       <c r="F52" s="6"/>
-      <c r="N52" s="6"/>
+      <c r="N52" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="O52" s="6"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1558,7 +1628,22 @@
       </c>
       <c r="F53" s="6"/>
       <c r="N53" s="6"/>
-      <c r="O53" s="6"/>
+      <c r="O53" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P53" s="0" t="n">
+        <v>10202767734</v>
+      </c>
+      <c r="Q53" s="0" t="n">
+        <f aca="false">P53-R53</f>
+        <v>7279455249</v>
+      </c>
+      <c r="R53" s="0" t="n">
+        <v>2923312485</v>
+      </c>
+      <c r="S53" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1"/>
@@ -1579,7 +1664,22 @@
       </c>
       <c r="F54" s="6"/>
       <c r="N54" s="6"/>
-      <c r="O54" s="6"/>
+      <c r="O54" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="P54" s="0" t="n">
+        <v>10202767734</v>
+      </c>
+      <c r="Q54" s="0" t="n">
+        <f aca="false">P54-R54</f>
+        <v>5045052543</v>
+      </c>
+      <c r="R54" s="0" t="n">
+        <v>5157715191</v>
+      </c>
+      <c r="S54" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
@@ -1602,7 +1702,22 @@
       </c>
       <c r="F55" s="6"/>
       <c r="N55" s="6"/>
-      <c r="O55" s="6"/>
+      <c r="O55" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P55" s="0" t="n">
+        <v>10202767734</v>
+      </c>
+      <c r="Q55" s="0" t="n">
+        <f aca="false">P55-R55</f>
+        <v>6682704349</v>
+      </c>
+      <c r="R55" s="0" t="n">
+        <v>3520063385</v>
+      </c>
+      <c r="S55" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1"/>
@@ -1622,7 +1737,9 @@
         <v>0.000134228372977381</v>
       </c>
       <c r="F56" s="6"/>
-      <c r="N56" s="6"/>
+      <c r="N56" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="O56" s="6"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1644,7 +1761,22 @@
       </c>
       <c r="F57" s="6"/>
       <c r="N57" s="6"/>
-      <c r="O57" s="6"/>
+      <c r="O57" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P57" s="0" t="n">
+        <v>3079415632</v>
+      </c>
+      <c r="Q57" s="0" t="n">
+        <f aca="false">P57-R57</f>
+        <v>2777331430</v>
+      </c>
+      <c r="R57" s="0" t="n">
+        <v>302084202</v>
+      </c>
+      <c r="S57" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1"/>
@@ -1665,7 +1797,22 @@
       </c>
       <c r="F58" s="6"/>
       <c r="N58" s="6"/>
-      <c r="O58" s="6"/>
+      <c r="O58" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="P58" s="0" t="n">
+        <v>3079415632</v>
+      </c>
+      <c r="Q58" s="0" t="n">
+        <f aca="false">P58-R58</f>
+        <v>2527207846</v>
+      </c>
+      <c r="R58" s="0" t="n">
+        <v>552207786</v>
+      </c>
+      <c r="S58" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
@@ -1688,7 +1835,22 @@
       </c>
       <c r="F59" s="6"/>
       <c r="N59" s="6"/>
-      <c r="O59" s="6"/>
+      <c r="O59" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P59" s="0" t="n">
+        <v>3079415632</v>
+      </c>
+      <c r="Q59" s="0" t="n">
+        <f aca="false">P59-R59</f>
+        <v>3025248687</v>
+      </c>
+      <c r="R59" s="0" t="n">
+        <v>54166945</v>
+      </c>
+      <c r="S59" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1"/>
@@ -1708,7 +1870,9 @@
         <v>0.29680934871702</v>
       </c>
       <c r="F60" s="6"/>
-      <c r="N60" s="6"/>
+      <c r="N60" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="O60" s="6"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1730,7 +1894,22 @@
       </c>
       <c r="F61" s="6"/>
       <c r="N61" s="6"/>
-      <c r="O61" s="6"/>
+      <c r="O61" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P61" s="0" t="n">
+        <v>6401505120</v>
+      </c>
+      <c r="Q61" s="0" t="n">
+        <f aca="false">P61-R61</f>
+        <v>4549678295</v>
+      </c>
+      <c r="R61" s="0" t="n">
+        <v>1851826825</v>
+      </c>
+      <c r="S61" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1"/>
@@ -1751,7 +1930,217 @@
       </c>
       <c r="F62" s="6"/>
       <c r="N62" s="6"/>
-      <c r="O62" s="6"/>
+      <c r="O62" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="P62" s="0" t="n">
+        <v>6401505120</v>
+      </c>
+      <c r="Q62" s="0" t="n">
+        <f aca="false">P62-R62</f>
+        <v>3100143151</v>
+      </c>
+      <c r="R62" s="0" t="n">
+        <v>3301361969</v>
+      </c>
+      <c r="S62" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O63" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="P63" s="0" t="n">
+        <v>6401505120</v>
+      </c>
+      <c r="Q63" s="0" t="n">
+        <f aca="false">P63-R63</f>
+        <v>4899360247</v>
+      </c>
+      <c r="R63" s="0" t="n">
+        <v>1502144873</v>
+      </c>
+      <c r="S63" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N64" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O65" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="P65" s="0" t="n">
+        <v>13506897459</v>
+      </c>
+      <c r="Q65" s="0" t="n">
+        <f aca="false">P65-R65</f>
+        <v>10437208229</v>
+      </c>
+      <c r="R65" s="0" t="n">
+        <v>3069689230</v>
+      </c>
+      <c r="S65" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O66" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="P66" s="0" t="n">
+        <v>13506897459</v>
+      </c>
+      <c r="Q66" s="0" t="n">
+        <f aca="false">P66-R66</f>
+        <v>4517212205</v>
+      </c>
+      <c r="R66" s="0" t="n">
+        <v>8989685254</v>
+      </c>
+      <c r="S66" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O67" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="P67" s="0" t="n">
+        <v>13506897459</v>
+      </c>
+      <c r="Q67" s="0" t="n">
+        <f aca="false">P67-R67</f>
+        <v>9244315131</v>
+      </c>
+      <c r="R67" s="0" t="n">
+        <v>4262582328</v>
+      </c>
+      <c r="S67" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N68" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O69" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="P69" s="0" t="n">
+        <v>24690256810</v>
+      </c>
+      <c r="Q69" s="0" t="n">
+        <f aca="false">P69-R69</f>
+        <v>24686942677</v>
+      </c>
+      <c r="R69" s="0" t="n">
+        <v>3314133</v>
+      </c>
+      <c r="S69" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O70" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="P70" s="0" t="n">
+        <v>24690256810</v>
+      </c>
+      <c r="Q70" s="0" t="n">
+        <f aca="false">P70-R70</f>
+        <v>12346481823</v>
+      </c>
+      <c r="R70" s="0" t="n">
+        <v>12343774987</v>
+      </c>
+      <c r="S70" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O71" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="P71" s="0" t="n">
+        <v>24690256810</v>
+      </c>
+      <c r="Q71" s="0" t="n">
+        <f aca="false">P71-R71</f>
+        <v>24687099667</v>
+      </c>
+      <c r="R71" s="0" t="n">
+        <v>3157143</v>
+      </c>
+      <c r="S71" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N72" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O73" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="P73" s="0" t="n">
+        <v>182287976534</v>
+      </c>
+      <c r="Q73" s="0" t="n">
+        <f aca="false">P73-R73</f>
+        <v>128183200940</v>
+      </c>
+      <c r="R73" s="0" t="n">
+        <v>54104775594</v>
+      </c>
+      <c r="S73" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O74" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="P74" s="0" t="n">
+        <v>182287976534</v>
+      </c>
+      <c r="Q74" s="0" t="n">
+        <f aca="false">P74-R74</f>
+        <v>75257786444</v>
+      </c>
+      <c r="R74" s="0" t="n">
+        <v>107030190090</v>
+      </c>
+      <c r="S74" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O75" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="P75" s="0" t="n">
+        <v>182287976534</v>
+      </c>
+      <c r="Q75" s="0" t="n">
+        <f aca="false">P75-R75</f>
+        <v>128183216939</v>
+      </c>
+      <c r="R75" s="0" t="n">
+        <v>54104759595</v>
+      </c>
+      <c r="S75" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>